<commit_message>
10-03-2018 : BugFixed->Employee CostCode->Add New
</commit_message>
<xml_diff>
--- a/upload_template/EmpMaster_Upload.xlsx
+++ b/upload_template/EmpMaster_Upload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance\upload_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance-Kosi\Attendance - Kosi - JSAW\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>PACEHCEM01</t>
+  </si>
+  <si>
+    <t>BASIC</t>
+  </si>
+  <si>
+    <t>CONT</t>
+  </si>
+  <si>
+    <t>NRG</t>
   </si>
 </sst>
 </file>
@@ -600,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +642,7 @@
     <col min="31" max="31" width="28.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -727,8 +736,11 @@
       <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9999999</v>
       </c>
@@ -809,6 +821,98 @@
       </c>
       <c r="AC2" s="6" t="s">
         <v>44</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9999999</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF3">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>